<commit_message>
Some changes and README
</commit_message>
<xml_diff>
--- a/Feature's list.xlsx
+++ b/Feature's list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsantiago\Documents\GustavoPersonal\Administration-Help-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787BADC0-2C26-4554-829B-467F36FC7076}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9023E750-B922-45C3-9476-4EFB6146A1F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista" sheetId="1" r:id="rId1"/>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,7 +656,7 @@
     <col min="2" max="2" width="25.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="40.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.109375" style="3" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -761,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5AB4AC5-71D3-4CCC-8A64-BC0F2A79EBDC}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>